<commit_message>
update SP2D GUP 17
</commit_message>
<xml_diff>
--- a/DATABASE/Laporan Monitoring Kontrak.xlsx
+++ b/DATABASE/Laporan Monitoring Kontrak.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="329">
   <si>
     <t>Monitoring Kontrak</t>
   </si>
@@ -955,6 +955,54 @@
   <si>
     <t>14-NOV-22</t>
   </si>
+  <si>
+    <t>A/175.22008802/0/0</t>
+  </si>
+  <si>
+    <t>PT. BIGJEK APLIKASI MANDIRI</t>
+  </si>
+  <si>
+    <t>'07-NOV-22</t>
+  </si>
+  <si>
+    <t>'04-NOV-22</t>
+  </si>
+  <si>
+    <t>SPK-4211/PPK/BRSDM.1/XI/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Jasa Pengembangan Dashboard Data Center BRSDM</t>
+  </si>
+  <si>
+    <t>18-NOV-22</t>
+  </si>
+  <si>
+    <t>A/175.22008962/0/0</t>
+  </si>
+  <si>
+    <t>10-NOV-22</t>
+  </si>
+  <si>
+    <t>'08-NOV-22</t>
+  </si>
+  <si>
+    <t>SPK-3752/PPK/BRSDM.1/XI/2022</t>
+  </si>
+  <si>
+    <t>Pengadaan Mebelair Ruang Kepala BRSDM</t>
+  </si>
+  <si>
+    <t>16-NOV-22</t>
+  </si>
+  <si>
+    <t>A/175.22008963/0/0</t>
+  </si>
+  <si>
+    <t>SPK-3673/PPK/BRSDM.1/XI/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Pembuatan dan Pemasangan Funiture Joinery Ruang Sekretaris Kepala BRSDM</t>
+  </si>
 </sst>
 </file>
 
@@ -1793,10 +1841,10 @@
         <v>570000000</v>
       </c>
       <c r="N7">
-        <v>380000000</v>
+        <v>475000000</v>
       </c>
       <c r="O7">
-        <v>190000000</v>
+        <v>95000000</v>
       </c>
       <c r="P7"/>
       <c r="Q7"/>
@@ -5405,10 +5453,10 @@
         <v>155164000</v>
       </c>
       <c r="N50">
-        <v>43702750</v>
+        <v>80856500</v>
       </c>
       <c r="O50">
-        <v>111461250</v>
+        <v>74307500</v>
       </c>
       <c r="P50"/>
       <c r="Q50"/>
@@ -6077,10 +6125,10 @@
         <v>31500000</v>
       </c>
       <c r="N58">
+        <v>31500000</v>
+      </c>
+      <c r="O58">
         <v>0</v>
-      </c>
-      <c r="O58">
-        <v>31500000</v>
       </c>
       <c r="P58"/>
       <c r="Q58"/>
@@ -6161,10 +6209,10 @@
         <v>30000000</v>
       </c>
       <c r="N59">
+        <v>30000000</v>
+      </c>
+      <c r="O59">
         <v>0</v>
-      </c>
-      <c r="O59">
-        <v>30000000</v>
       </c>
       <c r="P59"/>
       <c r="Q59"/>
@@ -6793,21 +6841,51 @@
       <c r="AZ66"/>
     </row>
     <row r="67" spans="1:52">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="L67"/>
-      <c r="M67"/>
-      <c r="N67"/>
-      <c r="O67"/>
+      <c r="A67">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>626402</v>
+      </c>
+      <c r="C67" t="s">
+        <v>313</v>
+      </c>
+      <c r="D67" t="s">
+        <v>314</v>
+      </c>
+      <c r="E67" t="s">
+        <v>315</v>
+      </c>
+      <c r="F67" t="s">
+        <v>316</v>
+      </c>
+      <c r="G67" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" t="s">
+        <v>317</v>
+      </c>
+      <c r="I67" t="s">
+        <v>318</v>
+      </c>
+      <c r="J67">
+        <v>522191</v>
+      </c>
+      <c r="K67" t="s">
+        <v>316</v>
+      </c>
+      <c r="L67" t="s">
+        <v>319</v>
+      </c>
+      <c r="M67">
+        <v>99900000</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>99900000</v>
+      </c>
       <c r="P67"/>
       <c r="Q67"/>
       <c r="R67"/>
@@ -6847,21 +6925,51 @@
       <c r="AZ67"/>
     </row>
     <row r="68" spans="1:52">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-      <c r="M68"/>
-      <c r="N68"/>
-      <c r="O68"/>
+      <c r="A68">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>626402</v>
+      </c>
+      <c r="C68" t="s">
+        <v>320</v>
+      </c>
+      <c r="D68" t="s">
+        <v>250</v>
+      </c>
+      <c r="E68" t="s">
+        <v>321</v>
+      </c>
+      <c r="F68" t="s">
+        <v>322</v>
+      </c>
+      <c r="G68" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" t="s">
+        <v>323</v>
+      </c>
+      <c r="I68" t="s">
+        <v>324</v>
+      </c>
+      <c r="J68">
+        <v>532111</v>
+      </c>
+      <c r="K68" t="s">
+        <v>322</v>
+      </c>
+      <c r="L68" t="s">
+        <v>325</v>
+      </c>
+      <c r="M68">
+        <v>191440000</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>191440000</v>
+      </c>
       <c r="P68"/>
       <c r="Q68"/>
       <c r="R68"/>
@@ -6901,21 +7009,51 @@
       <c r="AZ68"/>
     </row>
     <row r="69" spans="1:52">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
-      <c r="J69"/>
-      <c r="K69"/>
-      <c r="L69"/>
-      <c r="M69"/>
-      <c r="N69"/>
-      <c r="O69"/>
+      <c r="A69">
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>626402</v>
+      </c>
+      <c r="C69" t="s">
+        <v>326</v>
+      </c>
+      <c r="D69" t="s">
+        <v>223</v>
+      </c>
+      <c r="E69" t="s">
+        <v>321</v>
+      </c>
+      <c r="F69" t="s">
+        <v>322</v>
+      </c>
+      <c r="G69" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69" t="s">
+        <v>327</v>
+      </c>
+      <c r="I69" t="s">
+        <v>328</v>
+      </c>
+      <c r="J69">
+        <v>533121</v>
+      </c>
+      <c r="K69" t="s">
+        <v>322</v>
+      </c>
+      <c r="L69" t="s">
+        <v>325</v>
+      </c>
+      <c r="M69">
+        <v>146381000</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>146381000</v>
+      </c>
       <c r="P69"/>
       <c r="Q69"/>
       <c r="R69"/>

</xml_diff>

<commit_message>
Update SP2D LS Non Kontraktual
SP2D LS Non Kontraktual telah terbit semua
</commit_message>
<xml_diff>
--- a/DATABASE/Laporan Monitoring Kontrak.xlsx
+++ b/DATABASE/Laporan Monitoring Kontrak.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="406">
   <si>
     <t>Monitoring Kontrak</t>
   </si>
@@ -1003,6 +1003,237 @@
   <si>
     <t>Pekerjaan Pembuatan dan Pemasangan Funiture Joinery Ruang Sekretaris Kepala BRSDM</t>
   </si>
+  <si>
+    <t>A/175.22009480/0/0</t>
+  </si>
+  <si>
+    <t>PT. ASTRIDO JAYA MOBILINDO</t>
+  </si>
+  <si>
+    <t>25-NOV-22</t>
+  </si>
+  <si>
+    <t>SPK.4651/PPK/BRSDM.01/XI/2022</t>
+  </si>
+  <si>
+    <t>Pengadaan Kendaraan Dinas Pimpinan pada Sekretariat BRSDM</t>
+  </si>
+  <si>
+    <t>'01-DEC-22</t>
+  </si>
+  <si>
+    <t>A/175.22009496/0/0</t>
+  </si>
+  <si>
+    <t>UPP-TPA KOPERASI PERENCANAAN</t>
+  </si>
+  <si>
+    <t>480/PPK.PUSDIK/PL.430/XI/2022</t>
+  </si>
+  <si>
+    <t>Pelaksanaan Tes TOEFL dan TPA</t>
+  </si>
+  <si>
+    <t>21-NOV-22</t>
+  </si>
+  <si>
+    <t>22-NOV-22</t>
+  </si>
+  <si>
+    <t>A/175.22009544/0/0</t>
+  </si>
+  <si>
+    <t>PT. SAKHA PRATAMA MANDIRI</t>
+  </si>
+  <si>
+    <t>28-NOV-22</t>
+  </si>
+  <si>
+    <t>24-NOV-22</t>
+  </si>
+  <si>
+    <t>SPK-4631/PPK/BRSDM.1/XI/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Jasa Perbaikan/Perawatan Lift dan Komponennya pada Sekretariat BRSDM</t>
+  </si>
+  <si>
+    <t>15-DEC-22</t>
+  </si>
+  <si>
+    <t>A/175.22009792/0/0</t>
+  </si>
+  <si>
+    <t>PT ALFABET INDO KREATIF</t>
+  </si>
+  <si>
+    <t>'05-DEC-22</t>
+  </si>
+  <si>
+    <t>30-NOV-22</t>
+  </si>
+  <si>
+    <t>507/PPK.PUSDIK/PL.430/XI/2022</t>
+  </si>
+  <si>
+    <t>Pengadaan Kalender Pusat Pendidikan KP</t>
+  </si>
+  <si>
+    <t>14-DEC-22</t>
+  </si>
+  <si>
+    <t>A/175.22009873/0/0</t>
+  </si>
+  <si>
+    <t>DIN LAW GROUP</t>
+  </si>
+  <si>
+    <t>'07-DEC-22</t>
+  </si>
+  <si>
+    <t>SPK-4533/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Jasa Konsultasi Hukum Kegiatan Prioritas BRSDM</t>
+  </si>
+  <si>
+    <t>19-DEC-22</t>
+  </si>
+  <si>
+    <t>A/175.22009874/0/0</t>
+  </si>
+  <si>
+    <t>PT. PROSPERITAS FORTUNA INDONESIA</t>
+  </si>
+  <si>
+    <t>'02-DEC-22</t>
+  </si>
+  <si>
+    <t>SPK-4652/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Jasa Rehab Ruang Rapat Sekretariat BRSDM</t>
+  </si>
+  <si>
+    <t>12-DEC-22</t>
+  </si>
+  <si>
+    <t>A/175.22009996/0/0</t>
+  </si>
+  <si>
+    <t>'08-DEC-22</t>
+  </si>
+  <si>
+    <t>SPK_4831/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Pembuatan Kalender BRSDM 2023</t>
+  </si>
+  <si>
+    <t>A/175.22010016/0/0</t>
+  </si>
+  <si>
+    <t>MIRAH SEGAR</t>
+  </si>
+  <si>
+    <t>522/PPK.PUSDIK/PL.430/XII/2022</t>
+  </si>
+  <si>
+    <t>Pelaksanaan Fullboard Meeting Kegiatan Rapat Koordinasi Tugas Belajar dan Izin Belajar Tahun 2022</t>
+  </si>
+  <si>
+    <t>'09-DEC-22</t>
+  </si>
+  <si>
+    <t>A/175.22010060/0/0</t>
+  </si>
+  <si>
+    <t>PT. NOVAL INDO PRATAMA</t>
+  </si>
+  <si>
+    <t>13-DEC-22</t>
+  </si>
+  <si>
+    <t>SPK-4832/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Rehab Ruang Selasar Kepala BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010136/0/0</t>
+  </si>
+  <si>
+    <t>PT. ARGA SINAR TERANG</t>
+  </si>
+  <si>
+    <t>SPK-4852/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Instalasi Listrik dan AC Ruang Rapat BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010137/0/0</t>
+  </si>
+  <si>
+    <t>PT. ARTA ANUGRAH SEJAHTERA</t>
+  </si>
+  <si>
+    <t>SPK-4853/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Pembuatan Dinding Partisi Area Ruang Rapat BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010138/0/0</t>
+  </si>
+  <si>
+    <t>PT. AULIA BERLIAN KONSTRUKSI</t>
+  </si>
+  <si>
+    <t>SPK-4854/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Rehab Lantai dan Plafon Area Ruang Rapat BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010177/0/0</t>
+  </si>
+  <si>
+    <t>16-DEC-22</t>
+  </si>
+  <si>
+    <t>SPK-4936/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Pembuatan WLL Panel Ruang Rapat BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010178/0/0</t>
+  </si>
+  <si>
+    <t>SPK-4937/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Pembuatan Logo dan Custom Cabinet Ruang Rapat BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010179/0/0</t>
+  </si>
+  <si>
+    <t>SPK-4935/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Pekerjaan Pintu dan Partisi Kaca Ruang Rapat BRSDM</t>
+  </si>
+  <si>
+    <t>A/175.22010180/0/0</t>
+  </si>
+  <si>
+    <t>SPK-4893/PPK/BRSDM.1/XII/2022</t>
+  </si>
+  <si>
+    <t>Jasa Konstruksi Audience Bench Ruang Rapat Utama</t>
+  </si>
 </sst>
 </file>
 
@@ -1841,10 +2072,10 @@
         <v>570000000</v>
       </c>
       <c r="N7">
-        <v>475000000</v>
+        <v>522500000</v>
       </c>
       <c r="O7">
-        <v>95000000</v>
+        <v>47500000</v>
       </c>
       <c r="P7"/>
       <c r="Q7"/>
@@ -2009,10 +2240,10 @@
         <v>2388908230</v>
       </c>
       <c r="N9">
-        <v>1921284428</v>
+        <v>2090992550</v>
       </c>
       <c r="O9">
-        <v>467623802</v>
+        <v>297915680</v>
       </c>
       <c r="P9"/>
       <c r="Q9"/>
@@ -4865,10 +5096,10 @@
         <v>1560587173</v>
       </c>
       <c r="N43">
-        <v>1144430800</v>
+        <v>1297948045</v>
       </c>
       <c r="O43">
-        <v>416156373</v>
+        <v>262639128</v>
       </c>
       <c r="P43"/>
       <c r="Q43"/>
@@ -5369,10 +5600,10 @@
         <v>395250000</v>
       </c>
       <c r="N49">
+        <v>395250000</v>
+      </c>
+      <c r="O49">
         <v>0</v>
-      </c>
-      <c r="O49">
-        <v>395250000</v>
       </c>
       <c r="P49"/>
       <c r="Q49"/>
@@ -5453,10 +5684,10 @@
         <v>155164000</v>
       </c>
       <c r="N50">
-        <v>80856500</v>
+        <v>118010250</v>
       </c>
       <c r="O50">
-        <v>74307500</v>
+        <v>37153750</v>
       </c>
       <c r="P50"/>
       <c r="Q50"/>
@@ -6713,10 +6944,10 @@
         <v>98346000</v>
       </c>
       <c r="N65">
+        <v>98346000</v>
+      </c>
+      <c r="O65">
         <v>0</v>
-      </c>
-      <c r="O65">
-        <v>98346000</v>
       </c>
       <c r="P65"/>
       <c r="Q65"/>
@@ -6797,10 +7028,10 @@
         <v>86802000</v>
       </c>
       <c r="N66">
+        <v>86802000</v>
+      </c>
+      <c r="O66">
         <v>0</v>
-      </c>
-      <c r="O66">
-        <v>86802000</v>
       </c>
       <c r="P66"/>
       <c r="Q66"/>
@@ -6881,10 +7112,10 @@
         <v>99900000</v>
       </c>
       <c r="N67">
+        <v>99900000</v>
+      </c>
+      <c r="O67">
         <v>0</v>
-      </c>
-      <c r="O67">
-        <v>99900000</v>
       </c>
       <c r="P67"/>
       <c r="Q67"/>
@@ -6965,10 +7196,10 @@
         <v>191440000</v>
       </c>
       <c r="N68">
+        <v>191440000</v>
+      </c>
+      <c r="O68">
         <v>0</v>
-      </c>
-      <c r="O68">
-        <v>191440000</v>
       </c>
       <c r="P68"/>
       <c r="Q68"/>
@@ -7049,10 +7280,10 @@
         <v>146381000</v>
       </c>
       <c r="N69">
+        <v>146381000</v>
+      </c>
+      <c r="O69">
         <v>0</v>
-      </c>
-      <c r="O69">
-        <v>146381000</v>
       </c>
       <c r="P69"/>
       <c r="Q69"/>
@@ -7093,21 +7324,51 @@
       <c r="AZ69"/>
     </row>
     <row r="70" spans="1:52">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-      <c r="J70"/>
-      <c r="K70"/>
-      <c r="L70"/>
-      <c r="M70"/>
-      <c r="N70"/>
-      <c r="O70"/>
+      <c r="A70">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>626402</v>
+      </c>
+      <c r="C70" t="s">
+        <v>329</v>
+      </c>
+      <c r="D70" t="s">
+        <v>330</v>
+      </c>
+      <c r="E70" t="s">
+        <v>331</v>
+      </c>
+      <c r="F70" t="s">
+        <v>331</v>
+      </c>
+      <c r="G70" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" t="s">
+        <v>332</v>
+      </c>
+      <c r="I70" t="s">
+        <v>333</v>
+      </c>
+      <c r="J70">
+        <v>532111</v>
+      </c>
+      <c r="K70" t="s">
+        <v>331</v>
+      </c>
+      <c r="L70" t="s">
+        <v>334</v>
+      </c>
+      <c r="M70">
+        <v>712785000</v>
+      </c>
+      <c r="N70">
+        <v>712785000</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
       <c r="P70"/>
       <c r="Q70"/>
       <c r="R70"/>
@@ -7147,21 +7408,51 @@
       <c r="AZ70"/>
     </row>
     <row r="71" spans="1:52">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
-      <c r="J71"/>
-      <c r="K71"/>
-      <c r="L71"/>
-      <c r="M71"/>
-      <c r="N71"/>
-      <c r="O71"/>
+      <c r="A71">
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>626402</v>
+      </c>
+      <c r="C71" t="s">
+        <v>335</v>
+      </c>
+      <c r="D71" t="s">
+        <v>336</v>
+      </c>
+      <c r="E71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F71" t="s">
+        <v>319</v>
+      </c>
+      <c r="G71" t="s">
+        <v>20</v>
+      </c>
+      <c r="H71" t="s">
+        <v>337</v>
+      </c>
+      <c r="I71" t="s">
+        <v>338</v>
+      </c>
+      <c r="J71">
+        <v>522191</v>
+      </c>
+      <c r="K71" t="s">
+        <v>339</v>
+      </c>
+      <c r="L71" t="s">
+        <v>340</v>
+      </c>
+      <c r="M71">
+        <v>139805500</v>
+      </c>
+      <c r="N71">
+        <v>139805500</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
       <c r="P71"/>
       <c r="Q71"/>
       <c r="R71"/>
@@ -7201,21 +7492,51 @@
       <c r="AZ71"/>
     </row>
     <row r="72" spans="1:52">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
-      <c r="J72"/>
-      <c r="K72"/>
-      <c r="L72"/>
-      <c r="M72"/>
-      <c r="N72"/>
-      <c r="O72"/>
+      <c r="A72">
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <v>626402</v>
+      </c>
+      <c r="C72" t="s">
+        <v>341</v>
+      </c>
+      <c r="D72" t="s">
+        <v>342</v>
+      </c>
+      <c r="E72" t="s">
+        <v>343</v>
+      </c>
+      <c r="F72" t="s">
+        <v>344</v>
+      </c>
+      <c r="G72" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" t="s">
+        <v>345</v>
+      </c>
+      <c r="I72" t="s">
+        <v>346</v>
+      </c>
+      <c r="J72">
+        <v>523121</v>
+      </c>
+      <c r="K72" t="s">
+        <v>344</v>
+      </c>
+      <c r="L72" t="s">
+        <v>347</v>
+      </c>
+      <c r="M72">
+        <v>98000000</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>98000000</v>
+      </c>
       <c r="P72"/>
       <c r="Q72"/>
       <c r="R72"/>
@@ -7255,21 +7576,51 @@
       <c r="AZ72"/>
     </row>
     <row r="73" spans="1:52">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73"/>
-      <c r="E73"/>
-      <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
-      <c r="J73"/>
-      <c r="K73"/>
-      <c r="L73"/>
-      <c r="M73"/>
-      <c r="N73"/>
-      <c r="O73"/>
+      <c r="A73">
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <v>626402</v>
+      </c>
+      <c r="C73" t="s">
+        <v>348</v>
+      </c>
+      <c r="D73" t="s">
+        <v>349</v>
+      </c>
+      <c r="E73" t="s">
+        <v>350</v>
+      </c>
+      <c r="F73" t="s">
+        <v>351</v>
+      </c>
+      <c r="G73" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" t="s">
+        <v>352</v>
+      </c>
+      <c r="I73" t="s">
+        <v>353</v>
+      </c>
+      <c r="J73">
+        <v>521111</v>
+      </c>
+      <c r="K73" t="s">
+        <v>351</v>
+      </c>
+      <c r="L73" t="s">
+        <v>354</v>
+      </c>
+      <c r="M73">
+        <v>62770500</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>62770500</v>
+      </c>
       <c r="P73"/>
       <c r="Q73"/>
       <c r="R73"/>
@@ -7309,21 +7660,51 @@
       <c r="AZ73"/>
     </row>
     <row r="74" spans="1:52">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="D74"/>
-      <c r="E74"/>
-      <c r="F74"/>
-      <c r="G74"/>
-      <c r="H74"/>
-      <c r="I74"/>
-      <c r="J74"/>
-      <c r="K74"/>
-      <c r="L74"/>
-      <c r="M74"/>
-      <c r="N74"/>
-      <c r="O74"/>
+      <c r="A74">
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <v>626402</v>
+      </c>
+      <c r="C74" t="s">
+        <v>355</v>
+      </c>
+      <c r="D74" t="s">
+        <v>356</v>
+      </c>
+      <c r="E74" t="s">
+        <v>357</v>
+      </c>
+      <c r="F74" t="s">
+        <v>334</v>
+      </c>
+      <c r="G74" t="s">
+        <v>20</v>
+      </c>
+      <c r="H74" t="s">
+        <v>358</v>
+      </c>
+      <c r="I74" t="s">
+        <v>359</v>
+      </c>
+      <c r="J74">
+        <v>522191</v>
+      </c>
+      <c r="K74" t="s">
+        <v>334</v>
+      </c>
+      <c r="L74" t="s">
+        <v>360</v>
+      </c>
+      <c r="M74">
+        <v>176000000</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>176000000</v>
+      </c>
       <c r="P74"/>
       <c r="Q74"/>
       <c r="R74"/>
@@ -7363,21 +7744,51 @@
       <c r="AZ74"/>
     </row>
     <row r="75" spans="1:52">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="D75"/>
-      <c r="E75"/>
-      <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
-      <c r="J75"/>
-      <c r="K75"/>
-      <c r="L75"/>
-      <c r="M75"/>
-      <c r="N75"/>
-      <c r="O75"/>
+      <c r="A75">
+        <v>71</v>
+      </c>
+      <c r="B75">
+        <v>626402</v>
+      </c>
+      <c r="C75" t="s">
+        <v>361</v>
+      </c>
+      <c r="D75" t="s">
+        <v>362</v>
+      </c>
+      <c r="E75" t="s">
+        <v>357</v>
+      </c>
+      <c r="F75" t="s">
+        <v>363</v>
+      </c>
+      <c r="G75" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" t="s">
+        <v>364</v>
+      </c>
+      <c r="I75" t="s">
+        <v>365</v>
+      </c>
+      <c r="J75">
+        <v>523111</v>
+      </c>
+      <c r="K75" t="s">
+        <v>363</v>
+      </c>
+      <c r="L75" t="s">
+        <v>366</v>
+      </c>
+      <c r="M75">
+        <v>89982000</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>89982000</v>
+      </c>
       <c r="P75"/>
       <c r="Q75"/>
       <c r="R75"/>
@@ -7417,21 +7828,51 @@
       <c r="AZ75"/>
     </row>
     <row r="76" spans="1:52">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="D76"/>
-      <c r="E76"/>
-      <c r="F76"/>
-      <c r="G76"/>
-      <c r="H76"/>
-      <c r="I76"/>
-      <c r="J76"/>
-      <c r="K76"/>
-      <c r="L76"/>
-      <c r="M76"/>
-      <c r="N76"/>
-      <c r="O76"/>
+      <c r="A76">
+        <v>72</v>
+      </c>
+      <c r="B76">
+        <v>626402</v>
+      </c>
+      <c r="C76" t="s">
+        <v>367</v>
+      </c>
+      <c r="D76" t="s">
+        <v>217</v>
+      </c>
+      <c r="E76" t="s">
+        <v>366</v>
+      </c>
+      <c r="F76" t="s">
+        <v>368</v>
+      </c>
+      <c r="G76" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" t="s">
+        <v>369</v>
+      </c>
+      <c r="I76" t="s">
+        <v>370</v>
+      </c>
+      <c r="J76">
+        <v>521111</v>
+      </c>
+      <c r="K76" t="s">
+        <v>368</v>
+      </c>
+      <c r="L76" t="s">
+        <v>347</v>
+      </c>
+      <c r="M76">
+        <v>109057000</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>109057000</v>
+      </c>
       <c r="P76"/>
       <c r="Q76"/>
       <c r="R76"/>
@@ -7471,21 +7912,51 @@
       <c r="AZ76"/>
     </row>
     <row r="77" spans="1:52">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="D77"/>
-      <c r="E77"/>
-      <c r="F77"/>
-      <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
-      <c r="J77"/>
-      <c r="K77"/>
-      <c r="L77"/>
-      <c r="M77"/>
-      <c r="N77"/>
-      <c r="O77"/>
+      <c r="A77">
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <v>626402</v>
+      </c>
+      <c r="C77" t="s">
+        <v>371</v>
+      </c>
+      <c r="D77" t="s">
+        <v>372</v>
+      </c>
+      <c r="E77" t="s">
+        <v>366</v>
+      </c>
+      <c r="F77" t="s">
+        <v>357</v>
+      </c>
+      <c r="G77" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" t="s">
+        <v>373</v>
+      </c>
+      <c r="I77" t="s">
+        <v>374</v>
+      </c>
+      <c r="J77">
+        <v>524119</v>
+      </c>
+      <c r="K77" t="s">
+        <v>357</v>
+      </c>
+      <c r="L77" t="s">
+        <v>375</v>
+      </c>
+      <c r="M77">
+        <v>110250000</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77">
+        <v>110250000</v>
+      </c>
       <c r="P77"/>
       <c r="Q77"/>
       <c r="R77"/>
@@ -7525,21 +7996,51 @@
       <c r="AZ77"/>
     </row>
     <row r="78" spans="1:52">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="D78"/>
-      <c r="E78"/>
-      <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
-      <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78"/>
-      <c r="M78"/>
-      <c r="N78"/>
-      <c r="O78"/>
+      <c r="A78">
+        <v>74</v>
+      </c>
+      <c r="B78">
+        <v>626402</v>
+      </c>
+      <c r="C78" t="s">
+        <v>376</v>
+      </c>
+      <c r="D78" t="s">
+        <v>377</v>
+      </c>
+      <c r="E78" t="s">
+        <v>378</v>
+      </c>
+      <c r="F78" t="s">
+        <v>368</v>
+      </c>
+      <c r="G78" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" t="s">
+        <v>379</v>
+      </c>
+      <c r="I78" t="s">
+        <v>380</v>
+      </c>
+      <c r="J78">
+        <v>523111</v>
+      </c>
+      <c r="K78" t="s">
+        <v>368</v>
+      </c>
+      <c r="L78" t="s">
+        <v>366</v>
+      </c>
+      <c r="M78">
+        <v>193150000</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>193150000</v>
+      </c>
       <c r="P78"/>
       <c r="Q78"/>
       <c r="R78"/>
@@ -7579,21 +8080,51 @@
       <c r="AZ78"/>
     </row>
     <row r="79" spans="1:52">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="D79"/>
-      <c r="E79"/>
-      <c r="F79"/>
-      <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
-      <c r="J79"/>
-      <c r="K79"/>
-      <c r="L79"/>
-      <c r="M79"/>
-      <c r="N79"/>
-      <c r="O79"/>
+      <c r="A79">
+        <v>75</v>
+      </c>
+      <c r="B79">
+        <v>626402</v>
+      </c>
+      <c r="C79" t="s">
+        <v>381</v>
+      </c>
+      <c r="D79" t="s">
+        <v>382</v>
+      </c>
+      <c r="E79" t="s">
+        <v>347</v>
+      </c>
+      <c r="F79" t="s">
+        <v>375</v>
+      </c>
+      <c r="G79" t="s">
+        <v>20</v>
+      </c>
+      <c r="H79" t="s">
+        <v>383</v>
+      </c>
+      <c r="I79" t="s">
+        <v>384</v>
+      </c>
+      <c r="J79">
+        <v>523121</v>
+      </c>
+      <c r="K79" t="s">
+        <v>375</v>
+      </c>
+      <c r="L79" t="s">
+        <v>354</v>
+      </c>
+      <c r="M79">
+        <v>196656000</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>196656000</v>
+      </c>
       <c r="P79"/>
       <c r="Q79"/>
       <c r="R79"/>
@@ -7633,21 +8164,51 @@
       <c r="AZ79"/>
     </row>
     <row r="80" spans="1:52">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
-      <c r="F80"/>
-      <c r="G80"/>
-      <c r="H80"/>
-      <c r="I80"/>
-      <c r="J80"/>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80"/>
-      <c r="N80"/>
-      <c r="O80"/>
+      <c r="A80">
+        <v>76</v>
+      </c>
+      <c r="B80">
+        <v>626402</v>
+      </c>
+      <c r="C80" t="s">
+        <v>385</v>
+      </c>
+      <c r="D80" t="s">
+        <v>386</v>
+      </c>
+      <c r="E80" t="s">
+        <v>347</v>
+      </c>
+      <c r="F80" t="s">
+        <v>375</v>
+      </c>
+      <c r="G80" t="s">
+        <v>20</v>
+      </c>
+      <c r="H80" t="s">
+        <v>387</v>
+      </c>
+      <c r="I80" t="s">
+        <v>388</v>
+      </c>
+      <c r="J80">
+        <v>523111</v>
+      </c>
+      <c r="K80" t="s">
+        <v>375</v>
+      </c>
+      <c r="L80" t="s">
+        <v>354</v>
+      </c>
+      <c r="M80">
+        <v>198918000</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>198918000</v>
+      </c>
       <c r="P80"/>
       <c r="Q80"/>
       <c r="R80"/>
@@ -7687,21 +8248,51 @@
       <c r="AZ80"/>
     </row>
     <row r="81" spans="1:52">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
-      <c r="J81"/>
-      <c r="K81"/>
-      <c r="L81"/>
-      <c r="M81"/>
-      <c r="N81"/>
-      <c r="O81"/>
+      <c r="A81">
+        <v>77</v>
+      </c>
+      <c r="B81">
+        <v>626402</v>
+      </c>
+      <c r="C81" t="s">
+        <v>389</v>
+      </c>
+      <c r="D81" t="s">
+        <v>390</v>
+      </c>
+      <c r="E81" t="s">
+        <v>347</v>
+      </c>
+      <c r="F81" t="s">
+        <v>375</v>
+      </c>
+      <c r="G81" t="s">
+        <v>20</v>
+      </c>
+      <c r="H81" t="s">
+        <v>391</v>
+      </c>
+      <c r="I81" t="s">
+        <v>392</v>
+      </c>
+      <c r="J81">
+        <v>523111</v>
+      </c>
+      <c r="K81" t="s">
+        <v>375</v>
+      </c>
+      <c r="L81" t="s">
+        <v>354</v>
+      </c>
+      <c r="M81">
+        <v>162456659</v>
+      </c>
+      <c r="N81">
+        <v>0</v>
+      </c>
+      <c r="O81">
+        <v>162456659</v>
+      </c>
       <c r="P81"/>
       <c r="Q81"/>
       <c r="R81"/>
@@ -7741,21 +8332,51 @@
       <c r="AZ81"/>
     </row>
     <row r="82" spans="1:52">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
-      <c r="J82"/>
-      <c r="K82"/>
-      <c r="L82"/>
-      <c r="M82"/>
-      <c r="N82"/>
-      <c r="O82"/>
+      <c r="A82">
+        <v>78</v>
+      </c>
+      <c r="B82">
+        <v>626402</v>
+      </c>
+      <c r="C82" t="s">
+        <v>393</v>
+      </c>
+      <c r="D82" t="s">
+        <v>390</v>
+      </c>
+      <c r="E82" t="s">
+        <v>394</v>
+      </c>
+      <c r="F82" t="s">
+        <v>347</v>
+      </c>
+      <c r="G82" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82" t="s">
+        <v>395</v>
+      </c>
+      <c r="I82" t="s">
+        <v>396</v>
+      </c>
+      <c r="J82">
+        <v>523111</v>
+      </c>
+      <c r="K82" t="s">
+        <v>347</v>
+      </c>
+      <c r="L82" t="s">
+        <v>360</v>
+      </c>
+      <c r="M82">
+        <v>191086500</v>
+      </c>
+      <c r="N82">
+        <v>0</v>
+      </c>
+      <c r="O82">
+        <v>191086500</v>
+      </c>
       <c r="P82"/>
       <c r="Q82"/>
       <c r="R82"/>
@@ -7795,21 +8416,51 @@
       <c r="AZ82"/>
     </row>
     <row r="83" spans="1:52">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="D83"/>
-      <c r="E83"/>
-      <c r="F83"/>
-      <c r="G83"/>
-      <c r="H83"/>
-      <c r="I83"/>
-      <c r="J83"/>
-      <c r="K83"/>
-      <c r="L83"/>
-      <c r="M83"/>
-      <c r="N83"/>
-      <c r="O83"/>
+      <c r="A83">
+        <v>79</v>
+      </c>
+      <c r="B83">
+        <v>626402</v>
+      </c>
+      <c r="C83" t="s">
+        <v>397</v>
+      </c>
+      <c r="D83" t="s">
+        <v>386</v>
+      </c>
+      <c r="E83" t="s">
+        <v>394</v>
+      </c>
+      <c r="F83" t="s">
+        <v>347</v>
+      </c>
+      <c r="G83" t="s">
+        <v>20</v>
+      </c>
+      <c r="H83" t="s">
+        <v>398</v>
+      </c>
+      <c r="I83" t="s">
+        <v>399</v>
+      </c>
+      <c r="J83">
+        <v>523111</v>
+      </c>
+      <c r="K83" t="s">
+        <v>347</v>
+      </c>
+      <c r="L83" t="s">
+        <v>360</v>
+      </c>
+      <c r="M83">
+        <v>141192000</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>141192000</v>
+      </c>
       <c r="P83"/>
       <c r="Q83"/>
       <c r="R83"/>
@@ -7849,21 +8500,51 @@
       <c r="AZ83"/>
     </row>
     <row r="84" spans="1:52">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
-      <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84"/>
-      <c r="I84"/>
-      <c r="J84"/>
-      <c r="K84"/>
-      <c r="L84"/>
-      <c r="M84"/>
-      <c r="N84"/>
-      <c r="O84"/>
+      <c r="A84">
+        <v>80</v>
+      </c>
+      <c r="B84">
+        <v>626402</v>
+      </c>
+      <c r="C84" t="s">
+        <v>400</v>
+      </c>
+      <c r="D84" t="s">
+        <v>382</v>
+      </c>
+      <c r="E84" t="s">
+        <v>394</v>
+      </c>
+      <c r="F84" t="s">
+        <v>347</v>
+      </c>
+      <c r="G84" t="s">
+        <v>20</v>
+      </c>
+      <c r="H84" t="s">
+        <v>401</v>
+      </c>
+      <c r="I84" t="s">
+        <v>402</v>
+      </c>
+      <c r="J84">
+        <v>523111</v>
+      </c>
+      <c r="K84" t="s">
+        <v>347</v>
+      </c>
+      <c r="L84" t="s">
+        <v>360</v>
+      </c>
+      <c r="M84">
+        <v>130101990</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>130101990</v>
+      </c>
       <c r="P84"/>
       <c r="Q84"/>
       <c r="R84"/>
@@ -7903,21 +8584,51 @@
       <c r="AZ84"/>
     </row>
     <row r="85" spans="1:52">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
-      <c r="J85"/>
-      <c r="K85"/>
-      <c r="L85"/>
-      <c r="M85"/>
-      <c r="N85"/>
-      <c r="O85"/>
+      <c r="A85">
+        <v>81</v>
+      </c>
+      <c r="B85">
+        <v>626402</v>
+      </c>
+      <c r="C85" t="s">
+        <v>403</v>
+      </c>
+      <c r="D85" t="s">
+        <v>377</v>
+      </c>
+      <c r="E85" t="s">
+        <v>394</v>
+      </c>
+      <c r="F85" t="s">
+        <v>378</v>
+      </c>
+      <c r="G85" t="s">
+        <v>20</v>
+      </c>
+      <c r="H85" t="s">
+        <v>404</v>
+      </c>
+      <c r="I85" t="s">
+        <v>405</v>
+      </c>
+      <c r="J85">
+        <v>523111</v>
+      </c>
+      <c r="K85" t="s">
+        <v>378</v>
+      </c>
+      <c r="L85" t="s">
+        <v>360</v>
+      </c>
+      <c r="M85">
+        <v>193584000</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>193584000</v>
+      </c>
       <c r="P85"/>
       <c r="Q85"/>
       <c r="R85"/>

</xml_diff>